<commit_message>
Update part selection and create design D01
</commit_message>
<xml_diff>
--- a/docs/bom.xlsx
+++ b/docs/bom.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Bill of Materials</t>
   </si>
@@ -50,32 +50,50 @@
     <t>Lens, NA 0.65</t>
   </si>
   <si>
-    <t>Wedged window</t>
-  </si>
-  <si>
     <t>Fiber connectors</t>
   </si>
   <si>
     <t>Electrical connectors</t>
   </si>
   <si>
-    <t>Diffraction grating, blazed,</t>
-  </si>
-  <si>
-    <t>PZT</t>
-  </si>
-  <si>
-    <t>Mirror mount (grating)</t>
-  </si>
-  <si>
     <t>Lens tube</t>
+  </si>
+  <si>
+    <t>GR13-1210</t>
+  </si>
+  <si>
+    <t>Thorlabs</t>
+  </si>
+  <si>
+    <t>Ruled reflective diffraction grating, 1200/mm, 1um blaze, 12.7x12.7x6mm</t>
+  </si>
+  <si>
+    <t>AFW</t>
+  </si>
+  <si>
+    <t>260 + GST</t>
+  </si>
+  <si>
+    <t>WW11050-C14</t>
+  </si>
+  <si>
+    <t>Wedged N-BK7 Laser Window, 1dia, AR Coated: 1047 - 1064 nm</t>
+  </si>
+  <si>
+    <t>Mirror mount (grating mount)</t>
+  </si>
+  <si>
+    <t>PA4FK</t>
+  </si>
+  <si>
+    <t>4 x Piezo chip, 150V, 3.6um, bare electrodes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +108,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -112,9 +137,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,15 +459,21 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -450,28 +482,55 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
       <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
         <v>12</v>
+      </c>
+      <c r="D10">
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Grating positioning and lens mount
</commit_message>
<xml_diff>
--- a/docs/bom.xlsx
+++ b/docs/bom.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Bill of Materials</t>
   </si>
@@ -114,12 +114,30 @@
       <t>Piezo chip, 150V, 3.6um, bare electrodes</t>
     </r>
   </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>1740-1053-012</t>
+  </si>
+  <si>
+    <t>1740 Grooves, 1053nm Holographic Grating, 12.5x12.5x6mm</t>
+  </si>
+  <si>
+    <t>SSI</t>
+  </si>
+  <si>
+    <t>41 deg</t>
+  </si>
+  <si>
+    <t>70 deg</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -163,8 +181,20 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF800000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,12 +203,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -186,20 +222,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFADADAD"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,12 +546,12 @@
     <col min="3" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -512,7 +565,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -526,50 +579,50 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="11">
         <v>34.299999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="11">
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:5" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="6">
         <v>85.5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
@@ -582,47 +635,80 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="8">
         <v>65</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="E9" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="8" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="8">
+        <v>85</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>11</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="C19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19">
+        <f>SUM(D4:D18)</f>
+        <v>553.79999999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update cad and todos
</commit_message>
<xml_diff>
--- a/docs/bom.xlsx
+++ b/docs/bom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Bill of Materials</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>AFW</t>
-  </si>
-  <si>
-    <t>260 + GST</t>
   </si>
   <si>
     <t>KMSS_M</t>
@@ -127,10 +124,7 @@
     <t>SSI</t>
   </si>
   <si>
-    <t>41 deg</t>
-  </si>
-  <si>
-    <t>70 deg</t>
+    <t>Amount</t>
   </si>
 </sst>
 </file>
@@ -533,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,12 +540,12 @@
     <col min="3" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -562,10 +556,13 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -575,140 +572,218 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>260</v>
+      </c>
+      <c r="F4">
+        <f>D4*E4</f>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="B5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="D5" s="11">
+        <v>1</v>
+      </c>
+      <c r="E5" s="11">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="F5:F17" si="0">D5*E5</f>
+        <v>34.299999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="11">
-        <v>34.299999999999997</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="B6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="C6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="11">
+        <v>1</v>
+      </c>
+      <c r="E6" s="11">
+        <v>133</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6">
+        <v>85.5</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>85.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="11">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="7" t="s">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>120</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="8">
+        <v>1</v>
+      </c>
+      <c r="E9" s="8">
+        <v>65</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="8" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="8">
+        <v>1</v>
+      </c>
+      <c r="E10" s="8">
+        <v>85</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>31</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="6">
-        <v>85.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="8">
-        <v>65</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="8" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="8">
-        <v>85</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="F12">
+        <f>D12*E12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="E19" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="C19" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19">
-        <f>SUM(D4:D18)</f>
-        <v>553.79999999999995</v>
+      <c r="F19">
+        <f>SUM(F4:F18)</f>
+        <v>906.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add locating recess on GM mount - B03 seleted as final design
</commit_message>
<xml_diff>
--- a/docs/bom.xlsx
+++ b/docs/bom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>Bill of Materials</t>
   </si>
@@ -33,6 +33,9 @@
     <t>Supplier</t>
   </si>
   <si>
+    <t>Amount</t>
+  </si>
+  <si>
     <t>Price</t>
   </si>
   <si>
@@ -60,6 +63,12 @@
     <t>Polaris™ Low Drift Ø1/2" Mirror Mount, 3 Low-Profile Hex Adjusters</t>
   </si>
   <si>
+    <t>C240TME-1064</t>
+  </si>
+  <si>
+    <t>f = 8.07 mm, NA = 0.5, Mounted Geltech Aspheric Lens, AR: 1064 nm</t>
+  </si>
+  <si>
     <t>WW11050-C14</t>
   </si>
   <si>
@@ -72,33 +81,20 @@
     <t>Ruled reflective diffraction grating, 1200/mm, 1um blaze, 12.7x12.7x6mm</t>
   </si>
   <si>
+    <t>1740-1053-012</t>
+  </si>
+  <si>
+    <t>1740 Grooves, 1053nm Holographic Grating, 12.5x12.5x6mm</t>
+  </si>
+  <si>
+    <t>SSI</t>
+  </si>
+  <si>
     <t>PA4FK</t>
   </si>
   <si>
-    <t>Fiber connectors</t>
-  </si>
-  <si>
-    <t>Electrical connectors</t>
-  </si>
-  <si>
-    <t>C240TME-1064</t>
-  </si>
-  <si>
-    <t>f = 8.07 mm, NA = 0.5, Mounted Geltech Aspheric Lens, AR: 1064 nm</t>
-  </si>
-  <si>
-    <t>Lens accessory</t>
-  </si>
-  <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">4 x </t>
+      <t>4 x</t>
     </r>
     <r>
       <rPr>
@@ -112,26 +108,32 @@
     </r>
   </si>
   <si>
+    <t>PCh150/10x10/2</t>
+  </si>
+  <si>
+    <t>10x10x2mm piezo chip, &gt;3um (bipolar)</t>
+  </si>
+  <si>
+    <t>Piezomechanik</t>
+  </si>
+  <si>
+    <t>Lens accessory</t>
+  </si>
+  <si>
+    <t>Fiber connectors</t>
+  </si>
+  <si>
+    <t>Electrical connectors</t>
+  </si>
+  <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>1740-1053-012</t>
-  </si>
-  <si>
-    <t>1740 Grooves, 1053nm Holographic Grating, 12.5x12.5x6mm</t>
-  </si>
-  <si>
-    <t>SSI</t>
-  </si>
-  <si>
-    <t>Amount</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -149,6 +151,14 @@
     </font>
     <font>
       <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
@@ -156,39 +166,21 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF800000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,13 +189,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor rgb="FFCCFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -229,30 +239,101 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFCCFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFADADAD"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDAE3F3"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFE699"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -530,7 +611,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,21 +637,21 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -579,82 +660,82 @@
         <v>260</v>
       </c>
       <c r="F4">
-        <f>D4*E4</f>
+        <f t="shared" ref="F4:F11" si="0">D4*E4</f>
         <v>260</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="12" t="s">
+    <row r="5" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="B5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="11">
+      <c r="C5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="13">
         <v>1</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="13">
         <v>34.299999999999997</v>
       </c>
-      <c r="F5">
-        <f t="shared" ref="F5:F17" si="0">D5*E5</f>
+      <c r="F5" s="13">
+        <f t="shared" si="0"/>
         <v>34.299999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+    <row r="6" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="11">
+      <c r="D6" s="13">
         <v>1</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="13">
         <v>133</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="15">
         <f t="shared" si="0"/>
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="6">
+    <row r="7" spans="1:6" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2">
         <v>1</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="2">
         <v>85.5</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <f t="shared" si="0"/>
         <v>85.5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>13</v>
+      <c r="A8" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -669,13 +750,13 @@
     </row>
     <row r="9" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D9" s="8">
         <v>1</v>
@@ -683,111 +764,119 @@
       <c r="E9" s="8">
         <v>65</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="8">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="8" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="8">
+        <v>21</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="11">
         <v>1</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="11">
         <v>85</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="12">
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="3" t="s">
+    <row r="11" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11">
-        <v>4</v>
-      </c>
-      <c r="E11">
+      <c r="B11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="5">
+        <v>2</v>
+      </c>
+      <c r="E11" s="5">
         <v>31</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="5">
         <f t="shared" si="0"/>
-        <v>124</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12">
-        <f>D12*E12</f>
-        <v>0</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="5">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
+        <f>D13*E13</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
+        <f>D14*E14</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
       <c r="F15">
-        <f t="shared" si="0"/>
+        <f>D15*E15</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
+      <c r="B16" s="7"/>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f>D16*E16</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F17">
-        <f t="shared" si="0"/>
+        <f>D17*E17</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="E19" s="4" t="s">
-        <v>24</v>
+      <c r="A19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="F19">
         <f>SUM(F4:F18)</f>
-        <v>906.8</v>
+        <v>844.8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>